<commit_message>
cập nhật file excel
</commit_message>
<xml_diff>
--- a/PhanMem/Data/Cat-Ngay.xlsx
+++ b/PhanMem/Data/Cat-Ngay.xlsx
@@ -241,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -249,35 +249,29 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -584,118 +578,118 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="11" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -717,13 +711,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G3:G4"/>
@@ -737,6 +724,13 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>